<commit_message>
Uploaded 11-May-2021 10:39:57 {/src/main/resources/com/wakandaspace/drools_price_model/UtilisationDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/UtilisationDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/UtilisationDecision.xlsx
@@ -1010,10 +1010,10 @@
     <t>After-demise compensation</t>
   </si>
   <si>
-    <t>getBenefit_group().getName().equals()</t>
-  </si>
-  <si>
-    <t>getName().equals()</t>
+    <t>getBenefit_group().getName()</t>
+  </si>
+  <si>
+    <t>getName()</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1556,7 @@
   <dimension ref="A1:I284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>